<commit_message>
Pontos de luz de iluminação distribuidos
</commit_message>
<xml_diff>
--- a/Planilha Projeto Elétrico.xlsx
+++ b/Planilha Projeto Elétrico.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReposInstalacao\Instalacao2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98BF180D-DF23-4D92-8BB1-76D31D5A4F6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332AF61F-2464-4B61-8922-73D10B60EC74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cargas da Instalação" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
   <si>
     <t>Dependência</t>
   </si>
@@ -538,7 +538,22 @@
     <t xml:space="preserve">Circulação </t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
+    <t xml:space="preserve">1 chuveiro </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Forno elétrico </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1 Lava Louça </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 Microondas típico </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  1 cooktop  </t>
+  </si>
+  <si>
+    <t>divide em 2?</t>
   </si>
 </sst>
 </file>
@@ -640,7 +655,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -665,6 +680,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="39">
     <border>
@@ -1140,7 +1161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -1296,7 +1317,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1375,18 +1401,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1408,12 +1434,20 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2260,10 +2294,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2275,97 +2309,97 @@
     <col min="6" max="7" width="13.42578125" customWidth="1"/>
     <col min="8" max="8" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="27.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
       <c r="M1" s="17"/>
     </row>
-    <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
       <c r="M2" s="38"/>
     </row>
-    <row r="3" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
-      <c r="B3" s="64" t="s">
+      <c r="B3" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
       <c r="M3" s="19"/>
     </row>
-    <row r="4" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="66" t="s">
+    <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="70" t="s">
+      <c r="D4" s="71" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="70" t="s">
+      <c r="E4" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="68"/>
-      <c r="G4" s="73" t="s">
+      <c r="F4" s="69"/>
+      <c r="G4" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="74"/>
-      <c r="I4" s="74"/>
-      <c r="J4" s="73" t="s">
+      <c r="H4" s="75"/>
+      <c r="I4" s="75"/>
+      <c r="J4" s="74" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="74"/>
-      <c r="L4" s="74"/>
-      <c r="M4" s="75"/>
-    </row>
-    <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="67"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="71"/>
-      <c r="D5" s="72"/>
+      <c r="K4" s="75"/>
+      <c r="L4" s="75"/>
+      <c r="M4" s="76"/>
+    </row>
+    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="68"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="73"/>
       <c r="E5" s="8" t="s">
         <v>60</v>
       </c>
@@ -2394,7 +2428,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="2" t="s">
         <v>72</v>
@@ -2407,25 +2441,30 @@
         <f>13.552</f>
         <v>13.552</v>
       </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97">
+      <c r="E6" s="59">
+        <v>160</v>
+      </c>
+      <c r="F6" s="59">
+        <f>E6</f>
+        <v>160</v>
+      </c>
+      <c r="G6" s="59">
         <f>ROUNDUP(D6/5,0)</f>
         <v>3</v>
       </c>
-      <c r="H6" s="97">
+      <c r="H6" s="59">
         <f>G6</f>
         <v>3</v>
       </c>
-      <c r="I6" s="97" t="s">
-        <v>85</v>
-      </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I6" s="59">
+        <v>300</v>
+      </c>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="59"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>73</v>
@@ -2438,622 +2477,839 @@
         <f>16.16</f>
         <v>16.16</v>
       </c>
-      <c r="E7" s="98"/>
-      <c r="F7" s="98"/>
-      <c r="G7" s="97">
+      <c r="E7" s="60">
+        <v>220</v>
+      </c>
+      <c r="F7" s="59">
+        <f t="shared" ref="F7:F21" si="0">E7</f>
+        <v>220</v>
+      </c>
+      <c r="G7" s="59">
         <f>ROUNDUP(D7/5,0)</f>
         <v>4</v>
       </c>
-      <c r="H7" s="97">
-        <f t="shared" ref="H7:H18" si="0">G7</f>
+      <c r="H7" s="59">
+        <f t="shared" ref="H7:H21" si="1">G7</f>
         <v>4</v>
       </c>
-      <c r="I7" s="98"/>
-      <c r="J7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="I7" s="60">
+        <v>400</v>
+      </c>
+      <c r="J7" s="60"/>
+      <c r="K7" s="60"/>
+      <c r="L7" s="60"/>
+      <c r="M7" s="60"/>
+    </row>
+    <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="98">
         <f>12.1486</f>
         <v>12.1486</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="98">
         <f>13.9951</f>
         <v>13.995100000000001</v>
       </c>
-      <c r="E8" s="98"/>
-      <c r="F8" s="98"/>
+      <c r="E8" s="98">
+        <v>160</v>
+      </c>
+      <c r="F8" s="98">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
       <c r="G8" s="98">
         <f>ROUNDUP(D8/3.5,0)</f>
         <v>4</v>
       </c>
-      <c r="H8" s="97">
+      <c r="H8" s="98">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="98">
+        <f xml:space="preserve"> 600*3+100</f>
+        <v>1900</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="K8" s="60">
+        <v>3200</v>
+      </c>
+      <c r="L8" s="60">
+        <v>1</v>
+      </c>
+      <c r="M8" s="60">
+        <f>K8/L8</f>
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="99"/>
+      <c r="C9" s="99"/>
+      <c r="D9" s="99"/>
+      <c r="E9" s="99"/>
+      <c r="F9" s="99"/>
+      <c r="G9" s="99"/>
+      <c r="H9" s="99"/>
+      <c r="I9" s="99"/>
+      <c r="J9" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="K9" s="60">
+        <v>2800</v>
+      </c>
+      <c r="L9" s="60">
+        <v>0.95</v>
+      </c>
+      <c r="M9" s="60">
+        <f t="shared" ref="M9:M17" si="2">K9/L9</f>
+        <v>2947.3684210526317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="99"/>
+      <c r="E10" s="99"/>
+      <c r="F10" s="99"/>
+      <c r="G10" s="99"/>
+      <c r="H10" s="99"/>
+      <c r="I10" s="99"/>
+      <c r="J10" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="K10" s="60">
+        <v>900</v>
+      </c>
+      <c r="L10" s="60">
+        <v>0.92</v>
+      </c>
+      <c r="M10" s="60">
+        <f t="shared" si="2"/>
+        <v>978.26086956521738</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="99"/>
+      <c r="C11" s="99"/>
+      <c r="D11" s="99"/>
+      <c r="E11" s="99"/>
+      <c r="F11" s="99"/>
+      <c r="G11" s="99"/>
+      <c r="H11" s="99"/>
+      <c r="I11" s="99"/>
+      <c r="J11" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" s="100">
+        <v>2000</v>
+      </c>
+      <c r="L11" s="100">
+        <v>0.8</v>
+      </c>
+      <c r="M11" s="60">
+        <f t="shared" si="2"/>
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="101" t="s">
+        <v>84</v>
+      </c>
+      <c r="C12" s="101">
+        <v>7.3387000000000002</v>
+      </c>
+      <c r="D12" s="101">
+        <f>15.6955</f>
+        <v>15.695499999999999</v>
+      </c>
+      <c r="E12" s="102">
+        <v>100</v>
+      </c>
+      <c r="F12" s="102">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I8" s="98"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="1">
-        <f>4.6261</f>
-        <v>4.6261000000000001</v>
-      </c>
-      <c r="D9" s="1">
-        <f>10.5288</f>
-        <v>10.5288</v>
-      </c>
-      <c r="E9" s="98"/>
-      <c r="F9" s="98"/>
-      <c r="G9" s="98">
+        <v>100</v>
+      </c>
+      <c r="G12" s="102">
         <v>1</v>
       </c>
-      <c r="H9" s="97">
-        <f t="shared" si="0"/>
+      <c r="H12" s="102">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I9" s="98"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
+      <c r="I12" s="102">
+        <v>100</v>
+      </c>
+      <c r="J12" s="102"/>
+      <c r="K12" s="102"/>
+      <c r="L12" s="102"/>
+      <c r="M12" s="102"/>
+      <c r="N12" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C13" s="1">
         <f>12.4725</f>
         <v>12.4725</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D13" s="1">
         <f>16.4</f>
         <v>16.399999999999999</v>
       </c>
-      <c r="E10" s="98"/>
-      <c r="F10" s="98"/>
-      <c r="G10" s="98">
-        <f>ROUNDUP(D10/5,0)</f>
+      <c r="E13" s="60">
+        <v>160</v>
+      </c>
+      <c r="F13" s="60">
+        <f t="shared" si="0"/>
+        <v>160</v>
+      </c>
+      <c r="G13" s="60">
+        <f>ROUNDUP(D13/5,0)</f>
         <v>4</v>
       </c>
-      <c r="H10" s="97">
-        <f t="shared" si="0"/>
+      <c r="H13" s="60">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I10" s="98"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="59" t="s">
+      <c r="I13" s="60">
+        <f>400</f>
+        <v>400</v>
+      </c>
+      <c r="J13" s="60"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="58" t="s">
         <v>76</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C14" s="1">
         <f>3.6516</f>
         <v>3.6516000000000002</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D14" s="1">
         <f>8.1049</f>
         <v>8.1049000000000007</v>
       </c>
-      <c r="E11" s="98"/>
-      <c r="F11" s="98"/>
-      <c r="G11" s="98">
+      <c r="E14" s="60">
+        <v>100</v>
+      </c>
+      <c r="F14" s="60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G14" s="60">
         <v>1</v>
       </c>
-      <c r="H11" s="97">
-        <f t="shared" si="0"/>
+      <c r="H14" s="60">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I11" s="98"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="I14" s="60">
+        <v>600</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="K14" s="60">
+        <f>6800</f>
+        <v>6800</v>
+      </c>
+      <c r="L14" s="60">
+        <v>1</v>
+      </c>
+      <c r="M14" s="60">
+        <f t="shared" si="2"/>
+        <v>6800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C15" s="1">
         <f>8.5253</f>
         <v>8.5252999999999997</v>
       </c>
-      <c r="D12">
+      <c r="D15" s="1">
         <f>11.683</f>
         <v>11.683</v>
       </c>
-      <c r="E12" s="98"/>
-      <c r="F12" s="98"/>
-      <c r="G12" s="98">
-        <f>ROUNDUP(D12/5,0)</f>
+      <c r="E15" s="60">
+        <v>100</v>
+      </c>
+      <c r="F15" s="60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G15" s="60">
+        <f>ROUNDUP(D15/5,0)</f>
         <v>3</v>
       </c>
-      <c r="H12" s="97">
-        <f t="shared" si="0"/>
+      <c r="H15" s="60">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I12" s="98"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
+      <c r="I15" s="60">
+        <f>3*100</f>
+        <v>300</v>
+      </c>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C16" s="1">
         <f>8.9418</f>
         <v>8.9418000000000006</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D16" s="1">
         <f>13.288</f>
         <v>13.288</v>
       </c>
-      <c r="E13" s="98"/>
-      <c r="F13" s="98"/>
-      <c r="G13" s="98">
-        <f>ROUNDUP(D13/5,0)</f>
+      <c r="E16" s="60">
+        <v>100</v>
+      </c>
+      <c r="F16" s="60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G16" s="60">
+        <f>ROUNDUP(D16/5,0)</f>
         <v>3</v>
       </c>
-      <c r="H13" s="97">
-        <f t="shared" si="0"/>
+      <c r="H16" s="60">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I13" s="98"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C14" s="1">
-        <f>3.6477</f>
-        <v>3.6476999999999999</v>
-      </c>
-      <c r="D14" s="1">
-        <f>8.103</f>
-        <v>8.1029999999999998</v>
-      </c>
-      <c r="E14" s="98"/>
-      <c r="F14" s="98"/>
-      <c r="G14" s="98">
-        <v>1</v>
-      </c>
-      <c r="H14" s="97">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I14" s="98"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="1">
-        <f>3.2925</f>
-        <v>3.2925</v>
-      </c>
-      <c r="D15" s="1">
-        <f>7.6975</f>
-        <v>7.6974999999999998</v>
-      </c>
-      <c r="E15" s="98"/>
-      <c r="F15" s="98"/>
-      <c r="G15" s="98">
-        <f>ROUNDUP(D15/3.5,0)</f>
-        <v>3</v>
-      </c>
-      <c r="H15" s="97">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I15" s="98"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C16" s="1">
-        <f>7.0572</f>
-        <v>7.0571999999999999</v>
-      </c>
-      <c r="D16" s="1">
-        <f>16.491</f>
-        <v>16.491</v>
-      </c>
-      <c r="E16" s="98"/>
-      <c r="F16" s="98"/>
-      <c r="G16" s="98">
-        <v>1</v>
-      </c>
-      <c r="H16" s="97">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="98"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+      <c r="I16" s="60">
+        <f>100*3</f>
+        <v>300</v>
+      </c>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+      <c r="L16" s="60"/>
+      <c r="M16" s="60"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C17" s="1">
-        <f>8.9123</f>
-        <v>8.9123000000000001</v>
+        <f>3.6477</f>
+        <v>3.6476999999999999</v>
       </c>
       <c r="D17" s="1">
-        <f>15.9012</f>
-        <v>15.901199999999999</v>
-      </c>
-      <c r="E17" s="98"/>
-      <c r="F17" s="98"/>
-      <c r="G17" s="98">
-        <f>ROUNDUP(D17/5,0)</f>
-        <v>4</v>
-      </c>
-      <c r="H17" s="97">
+        <f>8.103</f>
+        <v>8.1029999999999998</v>
+      </c>
+      <c r="E17" s="60">
+        <v>100</v>
+      </c>
+      <c r="F17" s="60">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I17" s="98"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+        <v>100</v>
+      </c>
+      <c r="G17" s="60">
+        <v>1</v>
+      </c>
+      <c r="H17" s="60">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I17" s="60">
+        <v>600</v>
+      </c>
+      <c r="J17" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="K17" s="60">
+        <v>6800</v>
+      </c>
+      <c r="L17" s="60">
+        <v>1</v>
+      </c>
+      <c r="M17" s="60">
+        <f t="shared" si="2"/>
+        <v>6800</v>
+      </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" s="1">
+        <f>3.2925</f>
+        <v>3.2925</v>
+      </c>
+      <c r="D18" s="1">
+        <f>7.6975</f>
+        <v>7.6974999999999998</v>
+      </c>
+      <c r="E18" s="60">
+        <v>100</v>
+      </c>
+      <c r="F18" s="60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G18" s="60">
+        <f>ROUNDUP(D18/3.5,0)</f>
+        <v>3</v>
+      </c>
+      <c r="H18" s="60">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="I18" s="60">
+        <f>3*600</f>
+        <v>1800</v>
+      </c>
+      <c r="J18" s="60"/>
+      <c r="K18" s="60"/>
+      <c r="L18" s="60"/>
+      <c r="M18" s="60"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="1">
+        <f>7.0572</f>
+        <v>7.0571999999999999</v>
+      </c>
+      <c r="D19" s="1">
+        <f>16.491</f>
+        <v>16.491</v>
+      </c>
+      <c r="E19" s="60">
+        <v>100</v>
+      </c>
+      <c r="F19" s="60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G19" s="60">
+        <v>1</v>
+      </c>
+      <c r="H19" s="60">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I19" s="60">
+        <v>100</v>
+      </c>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="103"/>
+      <c r="B20" s="103" t="s">
+        <v>82</v>
+      </c>
+      <c r="C20" s="103">
+        <f>8.9123</f>
+        <v>8.9123000000000001</v>
+      </c>
+      <c r="D20" s="103">
+        <f>15.9012</f>
+        <v>15.901199999999999</v>
+      </c>
+      <c r="E20" s="100">
+        <v>100</v>
+      </c>
+      <c r="F20" s="100">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G20" s="100">
+        <f>ROUNDUP(D20/5,0)</f>
+        <v>4</v>
+      </c>
+      <c r="H20" s="100">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I20" s="100">
+        <f>400</f>
+        <v>400</v>
+      </c>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="100"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C21" s="1">
         <f>4.05</f>
         <v>4.05</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D21" s="1">
         <f>8.7</f>
         <v>8.6999999999999993</v>
       </c>
-      <c r="E18" s="98"/>
-      <c r="F18" s="98"/>
-      <c r="G18" s="98">
+      <c r="E21" s="60">
+        <v>100</v>
+      </c>
+      <c r="F21" s="60">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G21" s="60">
         <v>1</v>
       </c>
-      <c r="H18" s="97">
-        <f t="shared" si="0"/>
+      <c r="H21" s="60">
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I18" s="98"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+      <c r="I21" s="60">
+        <f>100</f>
+        <v>100</v>
+      </c>
+      <c r="J21" s="60"/>
+      <c r="K21" s="60"/>
+      <c r="L21" s="60"/>
+      <c r="M21" s="60"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="A22" s="15"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+      <c r="F22" s="15"/>
+      <c r="G22" s="15"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+      <c r="A23" s="15"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="15"/>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+      <c r="F23" s="15"/>
+      <c r="G23" s="15"/>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+      <c r="A24" s="15"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+      <c r="F24" s="15"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
-      <c r="H25" s="1"/>
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+      <c r="A25" s="15"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+      <c r="H26" s="15"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="15"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="A27" s="15"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
+      <c r="F27" s="15"/>
+      <c r="G27" s="15"/>
+      <c r="H27" s="15"/>
+      <c r="I27" s="15"/>
+      <c r="J27" s="15"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15"/>
+      <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+      <c r="A28" s="15"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="15"/>
+      <c r="E28" s="15"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="15"/>
+      <c r="H28" s="15"/>
+      <c r="I28" s="15"/>
+      <c r="J28" s="15"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="15"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
-      <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="A29" s="15"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="15"/>
+      <c r="E29" s="15"/>
+      <c r="F29" s="15"/>
+      <c r="G29" s="15"/>
+      <c r="H29" s="15"/>
+      <c r="I29" s="15"/>
+      <c r="J29" s="15"/>
+      <c r="K29" s="15"/>
+      <c r="L29" s="15"/>
+      <c r="M29" s="15"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1"/>
-      <c r="M30" s="1"/>
+      <c r="A30" s="15"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
+      <c r="E30" s="15"/>
+      <c r="F30" s="15"/>
+      <c r="G30" s="15"/>
+      <c r="H30" s="15"/>
+      <c r="I30" s="15"/>
+      <c r="J30" s="15"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="15"/>
+      <c r="M30" s="15"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
+      <c r="A31" s="15"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="15"/>
+      <c r="D31" s="15"/>
+      <c r="E31" s="15"/>
+      <c r="F31" s="15"/>
+      <c r="G31" s="15"/>
+      <c r="H31" s="15"/>
+      <c r="I31" s="15"/>
+      <c r="J31" s="15"/>
+      <c r="K31" s="15"/>
+      <c r="L31" s="15"/>
+      <c r="M31" s="15"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
+      <c r="A32" s="15"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="15"/>
+      <c r="D32" s="15"/>
+      <c r="E32" s="15"/>
+      <c r="F32" s="15"/>
+      <c r="G32" s="15"/>
+      <c r="H32" s="15"/>
+      <c r="I32" s="15"/>
+      <c r="J32" s="15"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="15"/>
+      <c r="M32" s="15"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
+      <c r="A33" s="15"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15"/>
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+      <c r="K33" s="15"/>
+      <c r="L33" s="15"/>
+      <c r="M33" s="15"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1"/>
-      <c r="M34" s="1"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="15"/>
+      <c r="D34" s="15"/>
+      <c r="E34" s="15"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="15"/>
+      <c r="H34" s="15"/>
+      <c r="I34" s="15"/>
+      <c r="J34" s="15"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="15"/>
+      <c r="M34" s="15"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
+      <c r="A35" s="15"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="15"/>
+      <c r="D35" s="15"/>
+      <c r="E35" s="15"/>
+      <c r="F35" s="15"/>
+      <c r="G35" s="15"/>
+      <c r="H35" s="15"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="15"/>
+      <c r="K35" s="15"/>
+      <c r="L35" s="15"/>
+      <c r="M35" s="15"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1"/>
-      <c r="M36" s="1"/>
+      <c r="A36" s="15"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="15"/>
+      <c r="E36" s="15"/>
+      <c r="F36" s="15"/>
+      <c r="G36" s="15"/>
+      <c r="H36" s="15"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="15"/>
+      <c r="K36" s="15"/>
+      <c r="L36" s="15"/>
+      <c r="M36" s="15"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
+      <c r="A37" s="15"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="15"/>
+      <c r="D37" s="15"/>
+      <c r="E37" s="15"/>
+      <c r="F37" s="15"/>
+      <c r="G37" s="15"/>
+      <c r="H37" s="15"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="15"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="15"/>
+      <c r="B38" s="15"/>
+      <c r="C38" s="15"/>
+      <c r="D38" s="15"/>
+      <c r="E38" s="15"/>
+      <c r="F38" s="15"/>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="15"/>
+      <c r="K38" s="15"/>
+      <c r="L38" s="15"/>
+      <c r="M38" s="15"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A39" s="15"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="15"/>
+      <c r="D39" s="15"/>
+      <c r="E39" s="15"/>
+      <c r="F39" s="15"/>
+      <c r="G39" s="15"/>
+      <c r="H39" s="15"/>
+      <c r="I39" s="15"/>
+      <c r="J39" s="15"/>
+      <c r="K39" s="15"/>
+      <c r="L39" s="15"/>
+      <c r="M39" s="15"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A40" s="15"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="15"/>
+      <c r="D40" s="15"/>
+      <c r="E40" s="15"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="15"/>
+      <c r="H40" s="15"/>
+      <c r="I40" s="15"/>
+      <c r="J40" s="15"/>
+      <c r="K40" s="15"/>
+      <c r="L40" s="15"/>
+      <c r="M40" s="15"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="15"/>
+      <c r="E41" s="15"/>
+      <c r="F41" s="15"/>
+      <c r="G41" s="15"/>
+      <c r="H41" s="15"/>
+      <c r="I41" s="15"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="15"/>
+      <c r="L41" s="15"/>
+      <c r="M41" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="18">
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="I8:I11"/>
     <mergeCell ref="B1:L1"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B3:L3"/>
@@ -3066,7 +3322,7 @@
     <mergeCell ref="G4:I4"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
@@ -3094,13 +3350,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="80"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="81"/>
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
@@ -3109,15 +3365,15 @@
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="81"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="82"/>
       <c r="H2" s="37"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
@@ -3126,15 +3382,15 @@
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="82"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="83"/>
       <c r="H3" s="37"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
@@ -3143,15 +3399,15 @@
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="78"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="80"/>
+      <c r="G4" s="80"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
@@ -3213,7 +3469,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="83" t="s">
+      <c r="E8" s="84" t="s">
         <v>64</v>
       </c>
       <c r="F8" s="41"/>
@@ -3230,7 +3486,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="84"/>
+      <c r="E9" s="85"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="52"/>
@@ -3245,7 +3501,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E10" s="84"/>
+      <c r="E10" s="85"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="52"/>
@@ -3290,12 +3546,12 @@
       <c r="H15" s="52"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="85" t="s">
+      <c r="A16" s="86" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
       <c r="E16" s="54"/>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
@@ -3382,28 +3638,28 @@
       <c r="L21" s="28"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="76" t="s">
+      <c r="A22" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="76"/>
+      <c r="B22" s="77"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="76" t="s">
+      <c r="A23" s="77" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="76"/>
+      <c r="B23" s="77"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="76" t="s">
+      <c r="A24" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="76"/>
+      <c r="B24" s="77"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="76" t="s">
+      <c r="A25" s="77" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="76"/>
+      <c r="B25" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3450,144 +3706,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="61"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="61"/>
-      <c r="M1" s="61"/>
-      <c r="N1" s="61"/>
-      <c r="O1" s="61"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="61"/>
-      <c r="R1" s="61"/>
-      <c r="S1" s="80"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+      <c r="L1" s="62"/>
+      <c r="M1" s="62"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+      <c r="Q1" s="62"/>
+      <c r="R1" s="62"/>
+      <c r="S1" s="81"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="63"/>
-      <c r="K2" s="63"/>
-      <c r="L2" s="63"/>
-      <c r="M2" s="63"/>
-      <c r="N2" s="63"/>
-      <c r="O2" s="63"/>
-      <c r="P2" s="63"/>
-      <c r="Q2" s="63"/>
-      <c r="R2" s="63"/>
-      <c r="S2" s="81"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="M2" s="64"/>
+      <c r="N2" s="64"/>
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="64"/>
+      <c r="R2" s="64"/>
+      <c r="S2" s="82"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="63" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="63"/>
-      <c r="N3" s="63"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="63"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="63"/>
-      <c r="S3" s="81"/>
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="64"/>
+      <c r="M3" s="64"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="64"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
+      <c r="R3" s="64"/>
+      <c r="S3" s="82"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="87" t="s">
+      <c r="A4" s="89" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="86" t="s">
+      <c r="B4" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="86" t="s">
+      <c r="C4" s="90" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="86" t="s">
+      <c r="D4" s="90" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="86" t="s">
+      <c r="F4" s="90" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="86" t="s">
+      <c r="G4" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="87" t="s">
+      <c r="H4" s="89" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="87" t="s">
+      <c r="I4" s="89" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="87" t="s">
+      <c r="J4" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="87" t="s">
+      <c r="K4" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="86" t="s">
+      <c r="L4" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="87" t="s">
+      <c r="M4" s="89" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="89" t="s">
+      <c r="N4" s="88" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="89" t="s">
+      <c r="O4" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="89" t="s">
+      <c r="P4" s="88" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" s="88" t="s">
+      <c r="Q4" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="88"/>
-      <c r="S4" s="88"/>
+      <c r="R4" s="87"/>
+      <c r="S4" s="87"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="87"/>
-      <c r="B5" s="86"/>
-      <c r="C5" s="86"/>
-      <c r="D5" s="86"/>
-      <c r="E5" s="87"/>
-      <c r="F5" s="86"/>
-      <c r="G5" s="86"/>
-      <c r="H5" s="87"/>
-      <c r="I5" s="87"/>
-      <c r="J5" s="87"/>
-      <c r="K5" s="87"/>
-      <c r="L5" s="86"/>
-      <c r="M5" s="87"/>
-      <c r="N5" s="89"/>
-      <c r="O5" s="89"/>
-      <c r="P5" s="89"/>
+      <c r="A5" s="89"/>
+      <c r="B5" s="90"/>
+      <c r="C5" s="90"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="90"/>
+      <c r="H5" s="89"/>
+      <c r="I5" s="89"/>
+      <c r="J5" s="89"/>
+      <c r="K5" s="89"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="89"/>
+      <c r="N5" s="88"/>
+      <c r="O5" s="88"/>
+      <c r="P5" s="88"/>
       <c r="Q5" s="55" t="s">
         <v>57</v>
       </c>
@@ -4029,6 +4285,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
     <mergeCell ref="Q4:S4"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
@@ -4045,10 +4305,6 @@
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4077,81 +4333,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="61"/>
-      <c r="G1" s="61"/>
-      <c r="H1" s="61"/>
-      <c r="I1" s="61"/>
-      <c r="J1" s="80"/>
+      <c r="A1" s="61"/>
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="81"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="62" t="s">
+      <c r="A2" s="63" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="63"/>
-      <c r="I2" s="63"/>
-      <c r="J2" s="81"/>
+      <c r="B2" s="64"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="64"/>
+      <c r="J2" s="82"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="65"/>
-      <c r="D3" s="65"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="82"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="83"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="93" t="s">
+      <c r="A4" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="95" t="s">
+      <c r="B4" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="95" t="s">
+      <c r="C4" s="96" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="95" t="s">
+      <c r="D4" s="96" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="93" t="s">
+      <c r="E4" s="94" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="93" t="s">
+      <c r="F4" s="94" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="93" t="s">
+      <c r="G4" s="94" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="90" t="s">
+      <c r="H4" s="91" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="91"/>
-      <c r="J4" s="92"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="93"/>
     </row>
     <row r="5" spans="1:10" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="94"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="96"/>
-      <c r="D5" s="96"/>
-      <c r="E5" s="94"/>
-      <c r="F5" s="94"/>
-      <c r="G5" s="94"/>
+      <c r="A5" s="95"/>
+      <c r="B5" s="97"/>
+      <c r="C5" s="97"/>
+      <c r="D5" s="97"/>
+      <c r="E5" s="95"/>
+      <c r="F5" s="95"/>
+      <c r="G5" s="95"/>
       <c r="H5" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
Pontos de tomada distribuidos
</commit_message>
<xml_diff>
--- a/Planilha Projeto Elétrico.xlsx
+++ b/Planilha Projeto Elétrico.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ReposInstalacao\Instalacao2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{332AF61F-2464-4B61-8922-73D10B60EC74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151675CB-AE57-4937-A2FF-B76F84D623E4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Dependência</t>
   </si>
@@ -554,6 +554,9 @@
   </si>
   <si>
     <t>divide em 2?</t>
+  </si>
+  <si>
+    <t>1 ar condicionado</t>
   </si>
 </sst>
 </file>
@@ -1323,123 +1326,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1448,6 +1334,123 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2297,7 +2300,7 @@
   <dimension ref="A1:N41"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2319,87 +2322,87 @@
       <c r="A1" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
+      <c r="B1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
       <c r="M1" s="17"/>
     </row>
     <row r="2" spans="1:14" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36"/>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
       <c r="M2" s="38"/>
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="18"/>
-      <c r="B3" s="65" t="s">
+      <c r="B3" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="66"/>
-      <c r="K3" s="66"/>
-      <c r="L3" s="66"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="72"/>
+      <c r="K3" s="72"/>
+      <c r="L3" s="72"/>
       <c r="M3" s="19"/>
     </row>
     <row r="4" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="73" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="69" t="s">
+      <c r="B4" s="75" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="71" t="s">
+      <c r="C4" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="D4" s="71" t="s">
+      <c r="D4" s="77" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="71" t="s">
+      <c r="E4" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="69"/>
-      <c r="G4" s="74" t="s">
+      <c r="F4" s="75"/>
+      <c r="G4" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="75"/>
-      <c r="I4" s="75"/>
-      <c r="J4" s="74" t="s">
+      <c r="H4" s="81"/>
+      <c r="I4" s="81"/>
+      <c r="J4" s="80" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="75"/>
-      <c r="L4" s="75"/>
-      <c r="M4" s="76"/>
+      <c r="K4" s="81"/>
+      <c r="L4" s="81"/>
+      <c r="M4" s="82"/>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="68"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="73"/>
+      <c r="A5" s="74"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="79"/>
       <c r="E5" s="8" t="s">
         <v>60</v>
       </c>
@@ -2453,11 +2456,11 @@
         <v>3</v>
       </c>
       <c r="H6" s="59">
-        <f>G6</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I6" s="59">
-        <v>300</v>
+        <f>100*H6</f>
+        <v>600</v>
       </c>
       <c r="J6" s="59"/>
       <c r="K6" s="59"/>
@@ -2493,6 +2496,7 @@
         <v>4</v>
       </c>
       <c r="I7" s="60">
+        <f>100*H7</f>
         <v>400</v>
       </c>
       <c r="J7" s="60"/>
@@ -2502,33 +2506,33 @@
     </row>
     <row r="8" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="98" t="s">
+      <c r="B8" s="65" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="98">
+      <c r="C8" s="65">
         <f>12.1486</f>
         <v>12.1486</v>
       </c>
-      <c r="D8" s="98">
+      <c r="D8" s="65">
         <f>13.9951</f>
         <v>13.995100000000001</v>
       </c>
-      <c r="E8" s="98">
+      <c r="E8" s="65">
         <v>160</v>
       </c>
-      <c r="F8" s="98">
+      <c r="F8" s="65">
         <f t="shared" si="0"/>
         <v>160</v>
       </c>
-      <c r="G8" s="98">
+      <c r="G8" s="65">
         <f>ROUNDUP(D8/3.5,0)</f>
         <v>4</v>
       </c>
-      <c r="H8" s="98">
+      <c r="H8" s="65">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="98">
+      <c r="I8" s="65">
         <f xml:space="preserve"> 600*3+100</f>
         <v>1900</v>
       </c>
@@ -2548,14 +2552,14 @@
     </row>
     <row r="9" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
-      <c r="B9" s="99"/>
-      <c r="C9" s="99"/>
-      <c r="D9" s="99"/>
-      <c r="E9" s="99"/>
-      <c r="F9" s="99"/>
-      <c r="G9" s="99"/>
-      <c r="H9" s="99"/>
-      <c r="I9" s="99"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="66"/>
       <c r="J9" s="11" t="s">
         <v>87</v>
       </c>
@@ -2572,14 +2576,14 @@
     </row>
     <row r="10" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
-      <c r="B10" s="99"/>
-      <c r="C10" s="99"/>
-      <c r="D10" s="99"/>
-      <c r="E10" s="99"/>
-      <c r="F10" s="99"/>
-      <c r="G10" s="99"/>
-      <c r="H10" s="99"/>
-      <c r="I10" s="99"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
       <c r="J10" s="11" t="s">
         <v>88</v>
       </c>
@@ -2596,21 +2600,21 @@
     </row>
     <row r="11" spans="1:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="99"/>
-      <c r="G11" s="99"/>
-      <c r="H11" s="99"/>
-      <c r="I11" s="99"/>
+      <c r="B11" s="66"/>
+      <c r="C11" s="66"/>
+      <c r="D11" s="66"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="66"/>
+      <c r="G11" s="66"/>
+      <c r="H11" s="66"/>
+      <c r="I11" s="66"/>
       <c r="J11" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="K11" s="100">
+      <c r="K11" s="61">
         <v>2000</v>
       </c>
-      <c r="L11" s="100">
+      <c r="L11" s="61">
         <v>0.8</v>
       </c>
       <c r="M11" s="60">
@@ -2620,37 +2624,38 @@
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
-      <c r="B12" s="101" t="s">
+      <c r="B12" s="62" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="101">
+      <c r="C12" s="62">
         <v>7.3387000000000002</v>
       </c>
-      <c r="D12" s="101">
+      <c r="D12" s="62">
         <f>15.6955</f>
         <v>15.695499999999999</v>
       </c>
-      <c r="E12" s="102">
+      <c r="E12" s="63">
         <v>100</v>
       </c>
-      <c r="F12" s="102">
+      <c r="F12" s="63">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G12" s="102">
+      <c r="G12" s="63">
         <v>1</v>
       </c>
-      <c r="H12" s="102">
+      <c r="H12" s="63">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="I12" s="102">
+      <c r="I12" s="63">
+        <f>100*H12</f>
         <v>100</v>
       </c>
-      <c r="J12" s="102"/>
-      <c r="K12" s="102"/>
-      <c r="L12" s="102"/>
-      <c r="M12" s="102"/>
+      <c r="J12" s="63"/>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
       <c r="N12" t="s">
         <v>90</v>
       </c>
@@ -2684,10 +2689,12 @@
         <v>4</v>
       </c>
       <c r="I13" s="60">
-        <f>400</f>
+        <f>100*H13</f>
         <v>400</v>
       </c>
-      <c r="J13" s="60"/>
+      <c r="J13" s="60" t="s">
+        <v>91</v>
+      </c>
       <c r="K13" s="60"/>
       <c r="L13" s="60"/>
       <c r="M13" s="60"/>
@@ -2766,7 +2773,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="60">
-        <f>3*100</f>
+        <f>100*H15</f>
         <v>300</v>
       </c>
       <c r="J15" s="60"/>
@@ -2803,7 +2810,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="60">
-        <f>100*3</f>
+        <f>100*H16</f>
         <v>300</v>
       </c>
       <c r="J16" s="60"/>
@@ -2920,6 +2927,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="60">
+        <f>100*H19</f>
         <v>100</v>
       </c>
       <c r="J19" s="60"/>
@@ -2928,41 +2936,41 @@
       <c r="M19" s="60"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="103"/>
-      <c r="B20" s="103" t="s">
+      <c r="A20" s="64"/>
+      <c r="B20" s="64" t="s">
         <v>82</v>
       </c>
-      <c r="C20" s="103">
+      <c r="C20" s="64">
         <f>8.9123</f>
         <v>8.9123000000000001</v>
       </c>
-      <c r="D20" s="103">
+      <c r="D20" s="64">
         <f>15.9012</f>
         <v>15.901199999999999</v>
       </c>
-      <c r="E20" s="100">
+      <c r="E20" s="61">
         <v>100</v>
       </c>
-      <c r="F20" s="100">
+      <c r="F20" s="61">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="G20" s="100">
+      <c r="G20" s="61">
         <f>ROUNDUP(D20/5,0)</f>
         <v>4</v>
       </c>
-      <c r="H20" s="100">
+      <c r="H20" s="61">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I20" s="100">
-        <f>400</f>
+      <c r="I20" s="61">
+        <f>100*H20</f>
         <v>400</v>
       </c>
-      <c r="J20" s="100"/>
-      <c r="K20" s="100"/>
-      <c r="L20" s="100"/>
-      <c r="M20" s="100"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61"/>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
@@ -2992,7 +3000,7 @@
         <v>1</v>
       </c>
       <c r="I21" s="60">
-        <f>100</f>
+        <f>100*H21</f>
         <v>100</v>
       </c>
       <c r="J21" s="60"/>
@@ -3302,17 +3310,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="C8:C11"/>
-    <mergeCell ref="D8:D11"/>
-    <mergeCell ref="E8:E11"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="G8:G11"/>
-    <mergeCell ref="H8:H11"/>
-    <mergeCell ref="I8:I11"/>
-    <mergeCell ref="B1:L1"/>
-    <mergeCell ref="B2:L2"/>
-    <mergeCell ref="B3:L3"/>
     <mergeCell ref="A4:A5"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="C4:C5"/>
@@ -3320,6 +3317,17 @@
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="E4:F4"/>
     <mergeCell ref="G4:I4"/>
+    <mergeCell ref="G8:G11"/>
+    <mergeCell ref="H8:H11"/>
+    <mergeCell ref="I8:I11"/>
+    <mergeCell ref="B1:L1"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="C8:C11"/>
+    <mergeCell ref="D8:D11"/>
+    <mergeCell ref="E8:E11"/>
+    <mergeCell ref="F8:F11"/>
   </mergeCells>
   <pageMargins left="0.51181102362204722" right="0.51181102362204722" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
@@ -3350,13 +3358,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="81"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="87"/>
       <c r="H1" s="37"/>
       <c r="I1" s="37"/>
       <c r="J1" s="37"/>
@@ -3365,15 +3373,15 @@
       <c r="M1" s="15"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="82"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="88"/>
       <c r="H2" s="37"/>
       <c r="I2" s="37"/>
       <c r="J2" s="37"/>
@@ -3382,15 +3390,15 @@
       <c r="M2" s="15"/>
     </row>
     <row r="3" spans="1:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="83"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="89"/>
       <c r="H3" s="37"/>
       <c r="I3" s="37"/>
       <c r="J3" s="37"/>
@@ -3399,15 +3407,15 @@
       <c r="M3" s="15"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="84" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
+      <c r="B4" s="85"/>
+      <c r="C4" s="85"/>
+      <c r="D4" s="85"/>
+      <c r="E4" s="85"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="21" t="s">
@@ -3469,7 +3477,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E8" s="84" t="s">
+      <c r="E8" s="90" t="s">
         <v>64</v>
       </c>
       <c r="F8" s="41"/>
@@ -3486,7 +3494,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E9" s="85"/>
+      <c r="E9" s="91"/>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="H9" s="52"/>
@@ -3501,7 +3509,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E10" s="85"/>
+      <c r="E10" s="91"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
       <c r="H10" s="52"/>
@@ -3546,12 +3554,12 @@
       <c r="H15" s="52"/>
     </row>
     <row r="16" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="86" t="s">
+      <c r="A16" s="92" t="s">
         <v>65</v>
       </c>
-      <c r="B16" s="86"/>
-      <c r="C16" s="86"/>
-      <c r="D16" s="86"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="54"/>
       <c r="F16" s="42"/>
       <c r="G16" s="42"/>
@@ -3638,28 +3646,28 @@
       <c r="L21" s="28"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="77" t="s">
+      <c r="A22" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="77"/>
+      <c r="B22" s="83"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="77" t="s">
+      <c r="A23" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="77"/>
+      <c r="B23" s="83"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="77" t="s">
+      <c r="A24" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="77"/>
+      <c r="B24" s="83"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="77" t="s">
+      <c r="A25" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="B25" s="77"/>
+      <c r="B25" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -3706,144 +3714,144 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="81"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="87"/>
     </row>
     <row r="2" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="64"/>
-      <c r="K2" s="64"/>
-      <c r="L2" s="64"/>
-      <c r="M2" s="64"/>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="64"/>
-      <c r="R2" s="64"/>
-      <c r="S2" s="82"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="70"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="70"/>
+      <c r="R2" s="70"/>
+      <c r="S2" s="88"/>
     </row>
     <row r="3" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="69" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="64"/>
-      <c r="J3" s="64"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="64"/>
-      <c r="N3" s="64"/>
-      <c r="O3" s="64"/>
-      <c r="P3" s="64"/>
-      <c r="Q3" s="64"/>
-      <c r="R3" s="64"/>
-      <c r="S3" s="82"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
+      <c r="H3" s="70"/>
+      <c r="I3" s="70"/>
+      <c r="J3" s="70"/>
+      <c r="K3" s="70"/>
+      <c r="L3" s="70"/>
+      <c r="M3" s="70"/>
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="70"/>
+      <c r="R3" s="70"/>
+      <c r="S3" s="88"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="94" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="90" t="s">
+      <c r="B4" s="93" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="90" t="s">
+      <c r="C4" s="93" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="90" t="s">
+      <c r="D4" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="89" t="s">
+      <c r="E4" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="90" t="s">
+      <c r="F4" s="93" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="90" t="s">
+      <c r="G4" s="93" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="89" t="s">
+      <c r="H4" s="94" t="s">
         <v>17</v>
       </c>
-      <c r="I4" s="89" t="s">
+      <c r="I4" s="94" t="s">
         <v>16</v>
       </c>
-      <c r="J4" s="89" t="s">
+      <c r="J4" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="89" t="s">
+      <c r="K4" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="L4" s="90" t="s">
+      <c r="L4" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="M4" s="89" t="s">
+      <c r="M4" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="N4" s="88" t="s">
+      <c r="N4" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="O4" s="88" t="s">
+      <c r="O4" s="96" t="s">
         <v>54</v>
       </c>
-      <c r="P4" s="88" t="s">
+      <c r="P4" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="Q4" s="87" t="s">
+      <c r="Q4" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="R4" s="87"/>
-      <c r="S4" s="87"/>
+      <c r="R4" s="95"/>
+      <c r="S4" s="95"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="89"/>
-      <c r="B5" s="90"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="90"/>
-      <c r="E5" s="89"/>
-      <c r="F5" s="90"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="89"/>
-      <c r="K5" s="89"/>
-      <c r="L5" s="90"/>
-      <c r="M5" s="89"/>
-      <c r="N5" s="88"/>
-      <c r="O5" s="88"/>
-      <c r="P5" s="88"/>
+      <c r="A5" s="94"/>
+      <c r="B5" s="93"/>
+      <c r="C5" s="93"/>
+      <c r="D5" s="93"/>
+      <c r="E5" s="94"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="93"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="94"/>
+      <c r="K5" s="94"/>
+      <c r="L5" s="93"/>
+      <c r="M5" s="94"/>
+      <c r="N5" s="96"/>
+      <c r="O5" s="96"/>
+      <c r="P5" s="96"/>
       <c r="Q5" s="55" t="s">
         <v>57</v>
       </c>
@@ -4285,11 +4293,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:E5"/>
-    <mergeCell ref="Q4:S4"/>
     <mergeCell ref="A1:S1"/>
     <mergeCell ref="A2:S2"/>
     <mergeCell ref="A3:S3"/>
@@ -4305,6 +4308,11 @@
     <mergeCell ref="L4:L5"/>
     <mergeCell ref="F4:F5"/>
     <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:E5"/>
+    <mergeCell ref="Q4:S4"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.31496062992125984" top="0.78740157480314965" bottom="0.78740157480314965" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -4333,81 +4341,81 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="61"/>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="81"/>
+      <c r="A1" s="67"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="87"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="63" t="s">
+      <c r="A2" s="69" t="s">
         <v>52</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
-      <c r="H2" s="64"/>
-      <c r="I2" s="64"/>
-      <c r="J2" s="82"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="88"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65" t="s">
+      <c r="A3" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="66"/>
-      <c r="C3" s="66"/>
-      <c r="D3" s="66"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="66"/>
-      <c r="G3" s="66"/>
-      <c r="H3" s="66"/>
-      <c r="I3" s="66"/>
-      <c r="J3" s="83"/>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="72"/>
+      <c r="I3" s="72"/>
+      <c r="J3" s="89"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="94" t="s">
+      <c r="A4" s="100" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="102" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="96" t="s">
+      <c r="C4" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="96" t="s">
+      <c r="D4" s="102" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="94" t="s">
+      <c r="E4" s="100" t="s">
         <v>68</v>
       </c>
-      <c r="F4" s="94" t="s">
+      <c r="F4" s="100" t="s">
         <v>69</v>
       </c>
-      <c r="G4" s="94" t="s">
+      <c r="G4" s="100" t="s">
         <v>70</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="97" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="92"/>
-      <c r="J4" s="93"/>
+      <c r="I4" s="98"/>
+      <c r="J4" s="99"/>
     </row>
     <row r="5" spans="1:10" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="95"/>
-      <c r="B5" s="97"/>
-      <c r="C5" s="97"/>
-      <c r="D5" s="97"/>
-      <c r="E5" s="95"/>
-      <c r="F5" s="95"/>
-      <c r="G5" s="95"/>
+      <c r="A5" s="101"/>
+      <c r="B5" s="103"/>
+      <c r="C5" s="103"/>
+      <c r="D5" s="103"/>
+      <c r="E5" s="101"/>
+      <c r="F5" s="101"/>
+      <c r="G5" s="101"/>
       <c r="H5" s="5" t="s">
         <v>8</v>
       </c>

</xml_diff>